<commit_message>
first-five full text readings.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BA2E1B-9778-48DD-8567-21B10BD31FB9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F0899D-D8BA-447D-886F-583FFED295F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>variance.measure</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>fruit number</t>
+  </si>
+  <si>
+    <t>invasive moth have greater impact on cactus vital rates than native herbivorous insects, herbivores reduce cactus drought tolerance,  weather impacts cactus vitals</t>
+  </si>
+  <si>
+    <t>invasive moths bad for cacti, weatehr impacts cacti, weather (rain) bad for moths</t>
   </si>
 </sst>
 </file>
@@ -421,13 +433,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -513,6 +541,26 @@
       </c>
       <c r="AB1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+      <c r="S2">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready to talk about with collaborators
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F0899D-D8BA-447D-886F-583FFED295F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F85231-1C7D-42AD-BBDB-2FD8AA989115}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -43,12 +43,6 @@
     <t>ecosystem</t>
   </si>
   <si>
-    <t>method</t>
-  </si>
-  <si>
-    <t>paragdign</t>
-  </si>
-  <si>
     <t>hypothesis</t>
   </si>
   <si>
@@ -97,25 +91,46 @@
     <t>variance.control</t>
   </si>
   <si>
-    <t>p-value</t>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>variance.measure</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>fruit number</t>
-  </si>
-  <si>
-    <t>invasive moth have greater impact on cactus vital rates than native herbivorous insects, herbivores reduce cactus drought tolerance,  weather impacts cactus vitals</t>
-  </si>
-  <si>
-    <t>invasive moths bad for cacti, weatehr impacts cacti, weather (rain) bad for moths</t>
+    <t xml:space="preserve">Opuntia ficus-indica </t>
+  </si>
+  <si>
+    <t>plant variant</t>
+  </si>
+  <si>
+    <t>Hercules</t>
+  </si>
+  <si>
+    <t>Ntopia</t>
+  </si>
+  <si>
+    <t>Percent seed weight to fruit biomass</t>
+  </si>
+  <si>
+    <t>r-value</t>
+  </si>
+  <si>
+    <t>variance.measurement</t>
+  </si>
+  <si>
+    <t>35_x0003_202700</t>
+  </si>
+  <si>
+    <t>33_x0003_550900</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>There are differences between Ntopia and Hercules variants of cacti</t>
+  </si>
+  <si>
+    <t>Descriptive</t>
   </si>
 </sst>
 </file>
@@ -433,31 +448,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,39 +543,66 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>166</v>
+      </c>
+      <c r="B2">
+        <v>166.1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2">
-        <v>6</v>
-      </c>
-      <c r="S2">
-        <v>106</v>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="U2">
+        <v>7.7</v>
+      </c>
+      <c r="X2">
+        <v>0.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>